<commit_message>
This is it, with Asset Tracker
</commit_message>
<xml_diff>
--- a/AssetTracker.xlsx
+++ b/AssetTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\ArtCenter\2020.09_GD2\Wk10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Classes\Term 3\Game Dev 2\FA21-EGAM202-KevinSlackie-FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8475FD40-6EAE-4CE2-BA03-F91CBE9B1E18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D426B4D4-10BB-4561-9EF2-E1D8E838AF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6075" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Asset Name (file or bundle)</t>
   </si>
@@ -37,6 +37,90 @@
   </si>
   <si>
     <t>Licensing (if you made it, say "original")</t>
+  </si>
+  <si>
+    <t>Animated Pixel Adventurer</t>
+  </si>
+  <si>
+    <t>Player Sprite</t>
+  </si>
+  <si>
+    <t>rvros</t>
+  </si>
+  <si>
+    <t>Free Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slime Monster </t>
+  </si>
+  <si>
+    <t>Enemy Sprite</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">original </t>
+  </si>
+  <si>
+    <t>Player Attack Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player controls </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brackeys </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Use from Tutorial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player Movement Code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">me </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background Castle Sprite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health Bar Script </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI for hitPoints variables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slime Adjective Script </t>
+  </si>
+  <si>
+    <t>Determine Enemy stats and behaviors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slime Animations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changing Slime Sprite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player Animations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changing Player Sprite </t>
+  </si>
+  <si>
+    <t>sprite by rvros, animation controller by me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TextMesh Pro </t>
+  </si>
+  <si>
+    <t>Display Enemy Adjective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tim Handley, me </t>
   </si>
 </sst>
 </file>
@@ -378,21 +462,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="50.88671875" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,6 +488,146 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>